<commit_message>
germanized assignments, minor typo fixes
</commit_message>
<xml_diff>
--- a/excel/assignments/Assignment10a_Workbook.xlsx
+++ b/excel/assignments/Assignment10a_Workbook.xlsx
@@ -18,15 +18,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
-  <si>
-    <t>Homeroom #</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
   <si>
     <t>Gabriel</t>
   </si>
@@ -119,9 +110,6 @@
   </si>
   <si>
     <t>Hanlon</t>
-  </si>
-  <si>
-    <t>T-Shirt Size</t>
   </si>
   <si>
     <t>Nathan</t>
@@ -226,16 +214,28 @@
     <t>Wrong Amout</t>
   </si>
   <si>
-    <t>Total Orders By Date</t>
+    <t>Zimmer #</t>
   </si>
   <si>
-    <t>Date</t>
+    <t>Vorname</t>
   </si>
   <si>
-    <t>Orders</t>
+    <t>Nachname</t>
   </si>
   <si>
-    <t>Payment Method</t>
+    <t>T-Shirt Größe</t>
+  </si>
+  <si>
+    <t>Zahlungsmethode</t>
+  </si>
+  <si>
+    <t>Bestellungen nach Datum</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Bestellungen #</t>
   </si>
 </sst>
 </file>
@@ -534,9 +534,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>38101</xdr:colOff>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>714376</xdr:rowOff>
+      <xdr:rowOff>495300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
@@ -551,8 +551,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1171576" y="714376"/>
-          <a:ext cx="4781550" cy="133350"/>
+          <a:off x="1819275" y="495300"/>
+          <a:ext cx="4448176" cy="352426"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -595,7 +595,7 @@
               </a:solidFill>
               <a:effectLst/>
             </a:rPr>
-            <a:t>2013 T-Shirt Orders</a:t>
+            <a:t>2013 T-Shirt Bestellungen</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -12684,7 +12684,7 @@
   <dimension ref="A1:AD108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12695,7 +12695,8 @@
     <col min="5" max="5" width="19" style="3" customWidth="1"/>
     <col min="6" max="6" width="14.875" style="31" customWidth="1"/>
     <col min="7" max="7" width="19.75" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="17" width="9" style="11"/>
+    <col min="8" max="8" width="14.25" style="11" customWidth="1"/>
+    <col min="9" max="17" width="9" style="11"/>
     <col min="18" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
@@ -12708,23 +12709,23 @@
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H2" s="33"/>
       <c r="I2" s="29"/>
@@ -12746,25 +12747,25 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
@@ -12779,16 +12780,16 @@
         <v>105</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G4" s="28">
         <v>41369</v>
@@ -12806,19 +12807,19 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G5" s="28">
         <v>41376</v>
@@ -12836,19 +12837,19 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>29</v>
-      </c>
       <c r="E6" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G6" s="28">
         <v>41383</v>
@@ -12869,16 +12870,16 @@
         <v>105</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G7" s="28">
         <v>41390</v>
@@ -12899,16 +12900,16 @@
         <v>105</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
@@ -12920,19 +12921,19 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
@@ -12947,16 +12948,16 @@
         <v>105</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
@@ -12968,19 +12969,19 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
@@ -12995,16 +12996,16 @@
         <v>135</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
@@ -13019,16 +13020,16 @@
         <v>110</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
@@ -13043,16 +13044,16 @@
         <v>135</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
@@ -13067,16 +13068,16 @@
         <v>135</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="R15" s="11"/>
       <c r="S15" s="11"/>
@@ -13091,16 +13092,16 @@
         <v>105</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="R16" s="11"/>
       <c r="S16" s="11"/>
@@ -13115,16 +13116,16 @@
         <v>110</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="R17" s="11"/>
       <c r="S17" s="11"/>
@@ -13136,19 +13137,19 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="R18" s="11"/>
       <c r="S18" s="11"/>
@@ -13163,16 +13164,16 @@
         <v>135</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
@@ -13187,16 +13188,16 @@
         <v>135</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="R20" s="11"/>
       <c r="S20" s="11"/>
@@ -13208,19 +13209,19 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="R21" s="11"/>
       <c r="S21" s="11"/>
@@ -13232,19 +13233,19 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="R22" s="11"/>
       <c r="S22" s="11"/>
@@ -13259,16 +13260,16 @@
         <v>105</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="R23" s="11"/>
       <c r="S23" s="11"/>
@@ -13283,16 +13284,16 @@
         <v>110</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="R24" s="11"/>
       <c r="S24" s="11"/>
@@ -13304,19 +13305,19 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="R25" s="11"/>
       <c r="S25" s="11"/>
@@ -13331,16 +13332,16 @@
         <v>135</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="R26" s="11"/>
       <c r="S26" s="11"/>
@@ -13355,16 +13356,16 @@
         <v>110</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="R27" s="11"/>
       <c r="S27" s="11"/>
@@ -13376,19 +13377,19 @@
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="R28" s="11"/>
       <c r="S28" s="11"/>
@@ -13400,19 +13401,19 @@
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A29" s="23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="R29" s="11"/>
       <c r="S29" s="11"/>

</xml_diff>